<commit_message>
Modify projects and the js file of ho the project new line works
</commit_message>
<xml_diff>
--- a/Resume.xlsx
+++ b/Resume.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\website\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB839D8C-8739-4C9A-9F8E-9695ED7D0F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7523610E-7316-4FFC-8A7F-F31B5D3BF09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
@@ -139,46 +139,16 @@
     <t>GitHub Link</t>
   </si>
   <si>
-    <t>Side Scrolling Game</t>
-  </si>
-  <si>
-    <t>The project involved creating an engaging 2D side-scrolling game using Unreal Engine. Key features included game mechanics, level design, and characters.</t>
-  </si>
-  <si>
     <t>https://github.com/tigran338/2DGame</t>
-  </si>
-  <si>
-    <t>Checkers</t>
-  </si>
-  <si>
-    <t>Unity and C# used to develop a 3D checkers game featuring two unique gameplay modes: Standard and King Mode. The game incorporates an intricate checkers logic system, facilitating competitive gameplay for two participants on a single screen. The standout feature of the project was the innovative King Mode, where gameplay starts with all pieces as kings, introducing a new twist to the classic game.</t>
   </si>
   <si>
     <t>https://github.com/tigran338/Checkers</t>
   </si>
   <si>
-    <t>Tetris</t>
-  </si>
-  <si>
-    <t>The game was developed using C# and Visual Studio IDE. A graphical user interface was implemented, allowing players to interact with the game using various types of buttons.</t>
-  </si>
-  <si>
     <t>https://github.com/tigran338/Tetris</t>
   </si>
   <si>
-    <t>Visual Calculator</t>
-  </si>
-  <si>
-    <t>The visual calculator app featured a user-friendly GUI, designed using C# and Visual Studio IDE.</t>
-  </si>
-  <si>
     <t>https://github.com/tigran338/Calculator</t>
-  </si>
-  <si>
-    <t>Python Console Application Chat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Program in Python that acts as both client and server. Multiple users can connect and communicate with each other through TCP connections established by the program. Implemented functionalities like establishing new connections, listing all current connections, sending messages to specific connections, and terminating connections. Utilized Python's socket and threading modules to handle multiple client connections and enable concurrent communication. </t>
   </si>
   <si>
     <t>https://github.com/tigran338/Console-Application-Chat-Python</t>
@@ -237,6 +207,47 @@
 HTML
 CSS
 JavaScript</t>
+  </si>
+  <si>
+    <t>•	Developed the main character, integrating animation, collision, controls, and health/mana systems.
+•	Expanded gameplay experience by developing diverse enemies, including boss, melee, and projectile types.
+•	Designed unique, immersive maps using specialized assets for each, enhancing environmental variety.
+•	Contributed to team strategy, ensuring quality via feedback exchanges and collaborative meetings.</t>
+  </si>
+  <si>
+    <t>•	Designed and created detailed 3D assets for checker pieces, contributing to the game's visual elements.
+•	Programmed intricate checkers logic, controls, and UI, ensuring a seamless player experience.
+•	Innovated with a unique 'King Mode,' enhancing traditional gameplay with a creative twist.</t>
+  </si>
+  <si>
+    <t>•	Developed an interactive Tetris game from scratch using C# within the Visual Studio environment.
+•	Implemented a GUI with intuitive navigation, utilizing default buttons for game menu interactions.
+•	Engineered game logic, including figure control, difficulty customization, and real-time score calculation.
+•	Introduced a custom difficulty feature, allowing players to enhance game speed for a more challenging experience.</t>
+  </si>
+  <si>
+    <t>•	Crafted a Python chat app serving as both client and server for real-time, multi-user messaging and interaction.
+•	Integrated features for connection, personalized messaging, and session control.
+•	Utilized Python sockets and threading for concurrent client communication.</t>
+  </si>
+  <si>
+    <t>Visual Calculator (Visual Studio, C#)</t>
+  </si>
+  <si>
+    <t>Side Scrolling Game (Unreal Engine)</t>
+  </si>
+  <si>
+    <t>Checkers (Unity, C#)</t>
+  </si>
+  <si>
+    <t>Tetris (Visual Studio, C#)</t>
+  </si>
+  <si>
+    <t>•	Programmed a standard calculator application in C# featuring essential arithmetic operations.
+•	Implemented a clean, intuitive GUI using Visual Studio, promoting ease of use.</t>
+  </si>
+  <si>
+    <t>Console Application Chat (Python, Socket, Threads)</t>
   </si>
 </sst>
 </file>
@@ -7819,11 +7830,13 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="44.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="117" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" customWidth="1"/>
   </cols>
@@ -7839,59 +7852,59 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="8" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="10" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="5" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -12883,7 +12896,7 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -12895,18 +12908,18 @@
   <sheetData>
     <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -12916,10 +12929,10 @@
     </row>
     <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -12929,10 +12942,10 @@
     </row>
     <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -12942,10 +12955,10 @@
     </row>
     <row r="5" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -12955,18 +12968,18 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>